<commit_message>
commit de actualizacion de base electoral. actualice datos electorales en f de enlaces confiables. hice join al reves de modo de contar con toda la data de todas las elecciones aun cuando haya instancias "missing"
</commit_message>
<xml_diff>
--- a/data_cuali/ACTORES RELEVANTES debates datos.xlsx
+++ b/data_cuali/ACTORES RELEVANTES debates datos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3603" uniqueCount="1707">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3637" uniqueCount="1732">
   <si>
     <t xml:space="preserve">NOMBRE</t>
   </si>
@@ -5148,6 +5148,9 @@
     <t xml:space="preserve">ENTREVISTE 11 mayo 2021 a las 17:00 hs</t>
   </si>
   <si>
+    <t xml:space="preserve">Referente internacional</t>
+  </si>
+  <si>
     <t xml:space="preserve">Matt Diller</t>
   </si>
   <si>
@@ -5175,6 +5178,9 @@
     <t xml:space="preserve">ENTREVISTE 1 marzo de 2024</t>
   </si>
   <si>
+    <t xml:space="preserve">Academia, especialista en campañas electorales, periodsmo y comunicación política</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nos conocíamos por grupo de investigación. Contacté por correo</t>
   </si>
   <si>
@@ -5185,6 +5191,75 @@
   </si>
   <si>
     <t xml:space="preserve">Gabriel Vommaro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Legislador, firmante de proyecto. UCR / La Pampa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">franciscotorroba1@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Encontré correo googleando</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Francisco Torroba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENTREVISTE 2 de mayo 2024, 30 min por meet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diputado acompañante de proyecto de debates. No redactó. Intercambios fueron muy fluidos. Respondió rápidamente a correo. Ofreció nueva entrevista hacia 8/9 de mayo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asesora Legislativa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/ACoAAA6g7UYBHuxCZShBTtklZ4O1IWYXW5gaex8/?lipi=urn%3Ali%3Apage%3Ad_flagship3_notifications%3BW2i0SyhWRAOjdxFKSvSosQ%3D%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contacté vía linkedin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olivia Cuq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30/4/2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Respuesta en Linkedin: me derivó a otro contacto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asesora legislativa de legislador De Narvaez que impulsó proyecto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asesor Legislativa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/ACoAAArbBNABUehgIxJ6LRtrkSEPzqO_zEIILv8/?lipi=urn%3Ali%3Apage%3Ad_flagship3_notifications%3BW2i0SyhWRAOjdxFKSvSosQ%3D%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andrés Tittarelli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se ofreció a responder en diferido, por whastapp. Todavía esperando respuesta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asesor legislativo de Tonelli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asesor legislativo y posteriormente legislador</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/ACoAAAG1CXcB0FAlBDVFTBi-k1z1GQKg6DUiXu8/?lipi=urn%3Ali%3Apage%3Ad_flagship3_notifications%3BW2i0SyhWRAOjdxFKSvSosQ%3D%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">José Luis Patiño</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se ofreció a comentar en diferido, por linkedin. Todavía esperando respuesta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asesor legislativo de Bullrich y posteriormente diputado</t>
   </si>
 </sst>
 </file>
@@ -19449,10 +19524,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E37" activeCellId="0" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19934,22 +20009,25 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>1694</v>
+      </c>
       <c r="E25" s="38" t="s">
-        <v>1694</v>
+        <v>1695</v>
       </c>
       <c r="G25" s="28" t="s">
-        <v>1695</v>
+        <v>1696</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>1696</v>
+        <v>1697</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>659</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>1697</v>
+        <v>1698</v>
       </c>
       <c r="E26" s="0" t="s">
         <v>719</v>
@@ -19958,21 +20036,21 @@
         <v>45202</v>
       </c>
       <c r="G26" s="28" t="s">
-        <v>1698</v>
+        <v>1699</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>1699</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>1700</v>
+        <v>1701</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>205</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>1701</v>
+        <v>1702</v>
       </c>
       <c r="E27" s="0" t="s">
         <v>380</v>
@@ -19981,23 +20059,133 @@
         <v>45294</v>
       </c>
       <c r="G27" s="28" t="s">
-        <v>1702</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1703</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>1704</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>205</v>
+      </c>
       <c r="D28" s="0" t="s">
-        <v>1703</v>
+        <v>1705</v>
       </c>
       <c r="E28" s="0" t="s">
+        <v>1706</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
         <v>1704</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="0" t="s">
+        <v>205</v>
+      </c>
       <c r="D29" s="0" t="s">
-        <v>1705</v>
+        <v>1707</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>1706</v>
+        <v>1708</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>1709</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>1710</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>1711</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>1712</v>
+      </c>
+      <c r="F30" s="39" t="n">
+        <v>45327</v>
+      </c>
+      <c r="G30" s="28" t="s">
+        <v>1713</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>1714</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>1715</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>1716</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>1717</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>1718</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>1719</v>
+      </c>
+      <c r="G31" s="28" t="s">
+        <v>1720</v>
+      </c>
+      <c r="H31" s="0" t="s">
+        <v>1721</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>1722</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>1723</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>1717</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>1724</v>
+      </c>
+      <c r="G32" s="28" t="s">
+        <v>1725</v>
+      </c>
+      <c r="H32" s="0" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>1727</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>1728</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>1717</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>1729</v>
+      </c>
+      <c r="G33" s="28" t="s">
+        <v>1730</v>
+      </c>
+      <c r="H33" s="0" t="s">
+        <v>1731</v>
       </c>
     </row>
   </sheetData>
@@ -20015,6 +20203,7 @@
     <hyperlink ref="C16" r:id="rId11" display="marioelopez@yahoo.com"/>
     <hyperlink ref="C17" r:id="rId12" display="verorocha@gmail.com"/>
     <hyperlink ref="H19" r:id="rId13" display="https://www.repretel.com/contactenos/   costa rica varios debates con pocos datos contactar eventualmente"/>
+    <hyperlink ref="C31" r:id="rId14" display="https://www.linkedin.com/in/ACoAAA6g7UYBHuxCZShBTtklZ4O1IWYXW5gaex8/?lipi=urn%3Ali%3Apage%3Ad_flagship3_notifications%3BW2i0SyhWRAOjdxFKSvSosQ%3D%3D"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>